<commit_message>
Minor changes on the plots of each case
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Interventions/Roasting.xlsx
+++ b/CVX_Kenya/Interventions/Roasting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\Interventions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FFFC7D-D9DB-4ABF-B77F-18908143DDE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484EFCC9-F5FD-4FCC-ADF0-C4424BD2D89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="187">
   <si>
     <t>level_row</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>Countering final demand of roasted coffee</t>
+  </si>
+  <si>
+    <t>Roasted coffee (commodity)</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1183,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,11 +1207,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="C2" s="1">
-        <f>main!C4</f>
-        <v>401</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>